<commit_message>
Mise à jour Backlog
</commit_message>
<xml_diff>
--- a/Divers/Backlog.xlsx
+++ b/Divers/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GODOT\SopraGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Godot\SopraGame\Divers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Tache</t>
   </si>
@@ -36,23 +36,38 @@
     <t>Barre de vie : style mortal kombat X. fixe sur l'écran en haut (gauche P1, droite P2)</t>
   </si>
   <si>
-    <t>Relance de la partie : Affichage de la victoire du player. En attente de l'appuie sur la touche Entrée pour relancer
+    <t>Réorganiser l'architecture des dossiers</t>
+  </si>
+  <si>
+    <t>Qui</t>
+  </si>
+  <si>
+    <t>Fait</t>
+  </si>
+  <si>
+    <t>DRI</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Relance de la partie avec la touche Entree</t>
+  </si>
+  <si>
+    <t>Affichage de la victoire du player
 Le player qui a gagné peut continuer à s'amuser tant que la touche Entrée n'est pas saisie</t>
   </si>
   <si>
-    <t>Réorganiser l'architecture des dossiers</t>
-  </si>
-  <si>
-    <t>Qui</t>
-  </si>
-  <si>
-    <t>Fait</t>
-  </si>
-  <si>
-    <t>DRI</t>
-  </si>
-  <si>
-    <t>En cours</t>
+    <t>Ajouter des coups spéciaux</t>
+  </si>
+  <si>
+    <t>Ajouter un menu avant de jouer</t>
+  </si>
+  <si>
+    <t>Ajouter les munitions</t>
+  </si>
+  <si>
+    <t>Ajouter les fatality</t>
   </si>
 </sst>
 </file>
@@ -399,7 +414,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,10 +428,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -433,46 +448,60 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>

</xml_diff>

<commit_message>
Ajout Timer et modificationdu zoom en fin de partie
</commit_message>
<xml_diff>
--- a/Divers/Backlog.xlsx
+++ b/Divers/Backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Tache</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Ajouter menu paramètre (vie, graphismes, munitions)</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
   </si>
 </sst>
 </file>
@@ -454,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -462,20 +465,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="79.28515625" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -485,8 +489,11 @@
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30">
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -496,8 +503,9 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -507,15 +515,17 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -525,8 +535,9 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -536,8 +547,9 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -547,156 +559,187 @@
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>

</xml_diff>